<commit_message>
Ready for first test.
</commit_message>
<xml_diff>
--- a/test_data/resources/dwca_matrix_bacterioplankton.xlsx
+++ b/test_data/resources/dwca_matrix_bacterioplankton.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="687" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7920" tabRatio="687" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="dwc_columns" sheetId="12" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="301">
   <si>
     <t>shark_sample_id_md5</t>
   </si>
@@ -245,9 +245,6 @@
     <t>text</t>
   </si>
   <si>
-    <t>SMHI</t>
-  </si>
-  <si>
     <t>TAXA-</t>
   </si>
   <si>
@@ -791,9 +788,6 @@
     <t>CC0</t>
   </si>
   <si>
-    <t>data_holding_centre</t>
-  </si>
-  <si>
     <t>dataset_name</t>
   </si>
   <si>
@@ -839,30 +833,9 @@
     <t>visit_date</t>
   </si>
   <si>
-    <t>reported_station_name</t>
-  </si>
-  <si>
-    <t>visit_reported_latitude_dd</t>
-  </si>
-  <si>
-    <t>visit_reported_longitude_dd</t>
-  </si>
-  <si>
-    <t>sample_depth_m</t>
-  </si>
-  <si>
     <t>SHARK Bacterioplankton</t>
   </si>
   <si>
-    <t>sample_reported_latitude_dd</t>
-  </si>
-  <si>
-    <t>sample_reported_longitude_dd</t>
-  </si>
-  <si>
-    <t>New bact.</t>
-  </si>
-  <si>
     <t>counted_portions</t>
   </si>
   <si>
@@ -878,7 +851,79 @@
     <t>preservation_method_code</t>
   </si>
   <si>
-    <t>PreservationMethod</t>
+    <t>AnalysisMethodCode</t>
+  </si>
+  <si>
+    <t>platform_code</t>
+  </si>
+  <si>
+    <t>PlatformCode</t>
+  </si>
+  <si>
+    <t>VisitYear</t>
+  </si>
+  <si>
+    <t>sample_orderer_code</t>
+  </si>
+  <si>
+    <t>sample_project_code</t>
+  </si>
+  <si>
+    <t>monitoring_program_code</t>
+  </si>
+  <si>
+    <t>SampleProjectCode</t>
+  </si>
+  <si>
+    <t>MonitoringProgramCode</t>
+  </si>
+  <si>
+    <t>analytical_laboratory_code</t>
+  </si>
+  <si>
+    <t>analytical_laboratory_accreditated</t>
+  </si>
+  <si>
+    <t>AnalyticalLaboratoryCode</t>
+  </si>
+  <si>
+    <t>AnalyticalLaboratoryAccreditated</t>
+  </si>
+  <si>
+    <t>AnalysedBy</t>
+  </si>
+  <si>
+    <t>SamplingLaboratoryCode</t>
+  </si>
+  <si>
+    <t>SamplingLaboratoryAccreditated</t>
+  </si>
+  <si>
+    <t>sampling_laboratory_accreditated</t>
+  </si>
+  <si>
+    <t>PreservationMethodCode</t>
+  </si>
+  <si>
+    <t>SamplingLaboratoryName</t>
+  </si>
+  <si>
+    <t>delivery_orderer_code</t>
+  </si>
+  <si>
+    <t>sampling_laboratory_name_sv</t>
+  </si>
+  <si>
+    <t>sampling_laboratory_name_en</t>
+  </si>
+  <si>
+    <t>AnalyticalLaboratoryName</t>
+  </si>
+  <si>
+    <t>analytical_laboratory_name_en</t>
+  </si>
+  <si>
+    <t>analytical_laboratory_name_sv</t>
   </si>
 </sst>
 </file>
@@ -1230,8 +1275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H49" sqref="H49"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1243,57 +1288,57 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>182</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B6" t="s">
         <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1301,10 +1346,10 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1312,32 +1357,32 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1345,10 +1390,10 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1356,29 +1401,29 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C14" t="s">
         <v>38</v>
@@ -1389,7 +1434,7 @@
         <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C15" t="s">
         <v>40</v>
@@ -1397,10 +1442,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C16" t="s">
         <v>42</v>
@@ -1408,10 +1453,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C17" t="s">
         <v>44</v>
@@ -1419,26 +1464,26 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1446,7 +1491,7 @@
         <v>11</v>
       </c>
       <c r="B21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1454,15 +1499,15 @@
         <v>13</v>
       </c>
       <c r="B22" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B23" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -1470,7 +1515,7 @@
         <v>47</v>
       </c>
       <c r="B24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -1478,7 +1523,7 @@
         <v>48</v>
       </c>
       <c r="B25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -1486,7 +1531,7 @@
         <v>15</v>
       </c>
       <c r="B26" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1494,15 +1539,15 @@
         <v>17</v>
       </c>
       <c r="B27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -1518,15 +1563,15 @@
         <v>21</v>
       </c>
       <c r="B30" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -1551,12 +1596,12 @@
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
@@ -1566,27 +1611,27 @@
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
@@ -1606,12 +1651,12 @@
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
@@ -1628,18 +1673,18 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I69"/>
+  <dimension ref="A1:I84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I50" sqref="I50"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C83" sqref="C83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" customWidth="1"/>
     <col min="3" max="3" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" customWidth="1"/>
     <col min="5" max="5" width="23" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.7109375" bestFit="1" customWidth="1"/>
@@ -1649,28 +1694,28 @@
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>138</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>73</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -1678,856 +1723,992 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B3" t="s">
         <v>62</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>10</v>
+        <v>194</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B4" t="s">
         <v>62</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>271</v>
+        <v>47</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B5" t="s">
         <v>62</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>179</v>
-      </c>
-      <c r="B6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>179</v>
-      </c>
-      <c r="B7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>273</v>
+        <v>48</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>179</v>
-      </c>
-      <c r="B8" t="s">
-        <v>62</v>
+        <v>64</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="C8" t="s">
+        <v>75</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>178</v>
+      </c>
+      <c r="B10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>178</v>
+      </c>
+      <c r="B14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" s="2"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>178</v>
+      </c>
+      <c r="B15" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" s="2"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>178</v>
+      </c>
+      <c r="B16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F16" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>179</v>
-      </c>
-      <c r="B9" t="s">
-        <v>62</v>
-      </c>
-      <c r="C9" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>179</v>
-      </c>
-      <c r="B10" t="s">
-        <v>62</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="G16" s="2"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>178</v>
+      </c>
+      <c r="B18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" t="s">
         <v>11</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F18" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A11"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>179</v>
-      </c>
-      <c r="B12" t="s">
-        <v>62</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>178</v>
+      </c>
+      <c r="B20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" t="s">
         <v>15</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F20" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H12" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>179</v>
-      </c>
-      <c r="B13" t="s">
-        <v>62</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="G20" s="2"/>
+      <c r="H20" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>178</v>
+      </c>
+      <c r="B21" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" t="s">
         <v>17</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F21" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="3" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>179</v>
-      </c>
-      <c r="B14" t="s">
-        <v>62</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="G21" s="2"/>
+      <c r="H21" s="3" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>178</v>
+      </c>
+      <c r="B22" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" t="s">
         <v>21</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F22" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H14" s="3" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A15"/>
-    </row>
-    <row r="16" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="G16" s="1" t="s">
+      <c r="G22" s="2"/>
+      <c r="H22" s="3" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+    </row>
+    <row r="24" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24" s="2" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>184</v>
-      </c>
-      <c r="B23" t="s">
-        <v>62</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="G24" s="2"/>
+    </row>
+    <row r="25" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="G25" s="2"/>
+    </row>
+    <row r="26" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>183</v>
+      </c>
+      <c r="B27" t="s">
+        <v>62</v>
+      </c>
+      <c r="D27" t="s">
+        <v>155</v>
+      </c>
+      <c r="E27" t="s">
+        <v>172</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="G27" s="2"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>183</v>
+      </c>
+      <c r="B28" t="s">
+        <v>62</v>
+      </c>
+      <c r="D28" t="s">
         <v>156</v>
       </c>
-      <c r="E23" t="s">
-        <v>173</v>
-      </c>
-      <c r="F23" t="s">
+      <c r="F28" s="2" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>184</v>
-      </c>
-      <c r="B24" t="s">
-        <v>62</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="G28" s="2"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>183</v>
+      </c>
+      <c r="B29" t="s">
+        <v>62</v>
+      </c>
+      <c r="D29" t="s">
         <v>157</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F29" s="2" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>184</v>
-      </c>
-      <c r="B25" t="s">
-        <v>62</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="G29" s="2"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>183</v>
+      </c>
+      <c r="B30" t="s">
+        <v>62</v>
+      </c>
+      <c r="D30" t="s">
         <v>158</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F30" s="2" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>184</v>
-      </c>
-      <c r="B26" t="s">
-        <v>62</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="G30" s="2"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>183</v>
+      </c>
+      <c r="B31" t="s">
+        <v>62</v>
+      </c>
+      <c r="D31" t="s">
         <v>159</v>
-      </c>
-      <c r="F26" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>184</v>
-      </c>
-      <c r="B27" t="s">
-        <v>62</v>
-      </c>
-      <c r="D27" t="s">
-        <v>160</v>
-      </c>
-      <c r="E27" t="s">
-        <v>174</v>
-      </c>
-      <c r="F27" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>184</v>
-      </c>
-      <c r="B28" t="s">
-        <v>62</v>
-      </c>
-      <c r="D28" t="s">
-        <v>161</v>
-      </c>
-      <c r="F28" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>184</v>
-      </c>
-      <c r="B29" t="s">
-        <v>62</v>
-      </c>
-      <c r="D29" t="s">
-        <v>162</v>
-      </c>
-      <c r="E29" t="s">
-        <v>173</v>
-      </c>
-      <c r="F29" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>184</v>
-      </c>
-      <c r="B30" t="s">
-        <v>62</v>
-      </c>
-      <c r="D30" t="s">
-        <v>163</v>
-      </c>
-      <c r="E30" t="s">
-        <v>173</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>184</v>
-      </c>
-      <c r="B31" t="s">
-        <v>62</v>
-      </c>
-      <c r="D31" t="s">
-        <v>164</v>
       </c>
       <c r="E31" t="s">
         <v>173</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F31" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G31" s="2"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>183</v>
+      </c>
+      <c r="B32" t="s">
+        <v>62</v>
+      </c>
+      <c r="D32" t="s">
+        <v>160</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G32" s="2"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>183</v>
+      </c>
+      <c r="B33" t="s">
+        <v>62</v>
+      </c>
+      <c r="D33" t="s">
+        <v>161</v>
+      </c>
+      <c r="E33" t="s">
+        <v>172</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="G33" s="2"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>183</v>
+      </c>
+      <c r="B34" t="s">
+        <v>62</v>
+      </c>
+      <c r="D34" t="s">
+        <v>162</v>
+      </c>
+      <c r="E34" t="s">
+        <v>172</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="G34" s="2"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>183</v>
+      </c>
+      <c r="B35" t="s">
+        <v>62</v>
+      </c>
+      <c r="D35" t="s">
+        <v>163</v>
+      </c>
+      <c r="E35" t="s">
+        <v>172</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="G35" s="2"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>183</v>
+      </c>
+      <c r="B36" t="s">
+        <v>62</v>
+      </c>
+      <c r="D36" t="s">
+        <v>164</v>
+      </c>
+      <c r="F36" s="2" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>184</v>
-      </c>
-      <c r="B32" t="s">
-        <v>62</v>
-      </c>
-      <c r="D32" t="s">
+      <c r="G36" s="2"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>183</v>
+      </c>
+      <c r="B37" t="s">
+        <v>62</v>
+      </c>
+      <c r="D37" t="s">
         <v>165</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F37" s="2" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>184</v>
-      </c>
-      <c r="B33" t="s">
-        <v>62</v>
-      </c>
-      <c r="D33" t="s">
+      <c r="G37" s="2"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>183</v>
+      </c>
+      <c r="B38" t="s">
+        <v>62</v>
+      </c>
+      <c r="D38" t="s">
         <v>166</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F38" s="2" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>184</v>
-      </c>
-      <c r="B34" t="s">
-        <v>62</v>
-      </c>
-      <c r="D34" t="s">
+      <c r="G38" s="2"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>183</v>
+      </c>
+      <c r="B39" t="s">
+        <v>62</v>
+      </c>
+      <c r="D39" t="s">
         <v>167</v>
       </c>
-      <c r="F34" t="s">
+      <c r="E39" t="s">
+        <v>174</v>
+      </c>
+      <c r="F39" s="2" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>184</v>
-      </c>
-      <c r="B35" t="s">
-        <v>62</v>
-      </c>
-      <c r="D35" t="s">
+      <c r="G39" s="2"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>183</v>
+      </c>
+      <c r="B40" t="s">
+        <v>62</v>
+      </c>
+      <c r="D40" t="s">
         <v>168</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E40" t="s">
+        <v>174</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="G40" s="2"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>183</v>
+      </c>
+      <c r="B41" t="s">
+        <v>62</v>
+      </c>
+      <c r="D41" t="s">
+        <v>169</v>
+      </c>
+      <c r="E41" t="s">
         <v>175</v>
       </c>
-      <c r="F35" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>184</v>
-      </c>
-      <c r="B36" t="s">
-        <v>62</v>
-      </c>
-      <c r="D36" t="s">
-        <v>169</v>
-      </c>
-      <c r="E36" t="s">
-        <v>175</v>
-      </c>
-      <c r="F36" t="s">
+      <c r="F41" s="2" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>184</v>
-      </c>
-      <c r="B37" t="s">
-        <v>62</v>
-      </c>
-      <c r="D37" t="s">
+      <c r="G41" s="2"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>183</v>
+      </c>
+      <c r="B42" t="s">
+        <v>62</v>
+      </c>
+      <c r="D42" t="s">
         <v>170</v>
       </c>
-      <c r="E37" t="s">
-        <v>176</v>
-      </c>
-      <c r="F37" t="s">
+      <c r="F42" s="2" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>184</v>
-      </c>
-      <c r="B38" t="s">
-        <v>62</v>
-      </c>
-      <c r="D38" t="s">
+      <c r="G42" s="2"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>183</v>
+      </c>
+      <c r="B43" t="s">
+        <v>62</v>
+      </c>
+      <c r="D43" t="s">
         <v>171</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F43" s="2" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>184</v>
-      </c>
-      <c r="B39" t="s">
-        <v>62</v>
-      </c>
-      <c r="D39" t="s">
-        <v>172</v>
-      </c>
-      <c r="F39" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>179</v>
-      </c>
-      <c r="B41" t="s">
-        <v>62</v>
-      </c>
-      <c r="C41" t="s">
-        <v>195</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>179</v>
-      </c>
-      <c r="B42" t="s">
-        <v>62</v>
-      </c>
-      <c r="C42" t="s">
-        <v>47</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>179</v>
-      </c>
-      <c r="B43" t="s">
-        <v>62</v>
-      </c>
-      <c r="C43" t="s">
-        <v>48</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>179</v>
-      </c>
-      <c r="B44" t="s">
-        <v>62</v>
-      </c>
-      <c r="C44" t="s">
-        <v>46</v>
-      </c>
-      <c r="F44" t="s">
+      <c r="G43" s="2"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+    </row>
+    <row r="45" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="G45" s="2"/>
+    </row>
+    <row r="46" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="F46" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="G44" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>179</v>
-      </c>
-      <c r="B46" t="s">
-        <v>63</v>
-      </c>
-      <c r="C46" t="s">
-        <v>19</v>
-      </c>
-      <c r="F46" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>179</v>
-      </c>
-      <c r="B47" t="s">
-        <v>63</v>
-      </c>
-      <c r="C47" t="s">
-        <v>27</v>
-      </c>
-      <c r="F47" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G46" s="2"/>
+    </row>
+    <row r="47" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="3"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>179</v>
-      </c>
-      <c r="B48" t="s">
+        <v>178</v>
+      </c>
+      <c r="B48" s="3" t="s">
         <v>63</v>
       </c>
       <c r="C48" t="s">
-        <v>29</v>
-      </c>
-      <c r="F48" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>179</v>
-      </c>
-      <c r="B49" t="s">
-        <v>63</v>
-      </c>
-      <c r="C49" t="s">
-        <v>23</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="H49" s="3" t="s">
-        <v>24</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G48" s="2"/>
+      <c r="H48" s="1"/>
+    </row>
+    <row r="49" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="G49" s="2"/>
+      <c r="H49" s="1"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>179</v>
-      </c>
-      <c r="B50" t="s">
+        <v>178</v>
+      </c>
+      <c r="B50" s="3" t="s">
         <v>63</v>
       </c>
       <c r="C50" t="s">
-        <v>25</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="H50" s="3" t="s">
-        <v>26</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G50" s="2"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B51" t="s">
         <v>63</v>
       </c>
       <c r="C51" t="s">
-        <v>1</v>
-      </c>
-      <c r="F51" t="s">
-        <v>2</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G51" s="2"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B52" t="s">
         <v>63</v>
       </c>
       <c r="C52" t="s">
-        <v>3</v>
-      </c>
-      <c r="F52" t="s">
-        <v>4</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G52" s="2"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B53" t="s">
         <v>63</v>
       </c>
       <c r="C53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54"/>
+        <v>29</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G53" s="2"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>178</v>
+      </c>
+      <c r="B54" t="s">
+        <v>63</v>
+      </c>
+      <c r="C54" t="s">
+        <v>23</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G54" s="2"/>
+      <c r="H54" s="3"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>64</v>
-      </c>
-      <c r="B55" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B55" t="s">
         <v>63</v>
       </c>
       <c r="C55" t="s">
-        <v>36</v>
-      </c>
-      <c r="F55" t="s">
-        <v>37</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G55" s="2"/>
+      <c r="H55" s="3"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>64</v>
-      </c>
-      <c r="B56" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B56" t="s">
         <v>63</v>
       </c>
       <c r="C56" t="s">
-        <v>86</v>
-      </c>
-      <c r="F56" t="s">
-        <v>87</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G56" s="2"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>64</v>
-      </c>
-      <c r="B57" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B57" t="s">
         <v>63</v>
       </c>
       <c r="C57" t="s">
-        <v>85</v>
-      </c>
-      <c r="F57" t="s">
-        <v>66</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G57" s="2"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>64</v>
-      </c>
-      <c r="B58" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B58" t="s">
         <v>63</v>
       </c>
       <c r="C58" t="s">
-        <v>76</v>
-      </c>
-      <c r="G58" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>184</v>
+        <v>13</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G58" s="2"/>
+    </row>
+    <row r="59" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="G59" s="2"/>
+    </row>
+    <row r="60" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="3" t="s">
+        <v>178</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D60" t="s">
-        <v>189</v>
-      </c>
-      <c r="E60" t="s">
-        <v>188</v>
-      </c>
-      <c r="F60" t="s">
-        <v>177</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="G60" s="2"/>
+    </row>
+    <row r="61" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="3"/>
+      <c r="E61" s="3"/>
+      <c r="F61" s="2"/>
+      <c r="G61" s="2"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>184</v>
+        <v>64</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C62" t="s">
-        <v>38</v>
-      </c>
-      <c r="F62" s="1" t="s">
-        <v>39</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G62" s="2"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>184</v>
+        <v>64</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C63" t="s">
-        <v>40</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>41</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G63" s="2"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>184</v>
+        <v>64</v>
       </c>
       <c r="B64" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C64" t="s">
+        <v>84</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G64" s="2"/>
+    </row>
+    <row r="65" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F65" s="2"/>
+      <c r="G65" s="2"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>183</v>
+      </c>
+      <c r="B66" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C64" t="s">
-        <v>42</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>184</v>
-      </c>
-      <c r="B65" s="3" t="s">
+      <c r="D66" t="s">
+        <v>188</v>
+      </c>
+      <c r="E66" t="s">
+        <v>187</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="G66" s="2"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>183</v>
+      </c>
+      <c r="B67" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C65" s="3" t="s">
+      <c r="C67" t="s">
+        <v>38</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G67" s="2"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>183</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C68" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="F65" s="1" t="s">
+      <c r="F68" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>228</v>
-      </c>
+      <c r="G68" s="2"/>
+    </row>
+    <row r="69" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G69" s="2"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G70" s="2"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G71" s="2"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>227</v>
+      </c>
+      <c r="G72" s="2"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G73" s="2"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G74" s="2"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G75" s="2"/>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G76" s="2"/>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G77" s="2"/>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G78" s="2"/>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G79" s="2"/>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G80" s="2"/>
+    </row>
+    <row r="81" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G81" s="2"/>
+    </row>
+    <row r="82" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G82" s="2"/>
+    </row>
+    <row r="83" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G83" s="2"/>
+    </row>
+    <row r="84" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G84" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -2539,8 +2720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q13"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1"/>
+    <sheetView topLeftCell="E1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2564,22 +2745,22 @@
   <sheetData>
     <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>254</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>52</v>
@@ -2612,12 +2793,12 @@
         <v>61</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B3" t="s">
         <v>62</v>
@@ -2640,7 +2821,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B5" t="s">
         <v>63</v>
@@ -2659,6 +2840,9 @@
       </c>
       <c r="G5" t="s">
         <v>0</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -2678,7 +2862,7 @@
         <v>70</v>
       </c>
       <c r="F7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G7" t="s">
         <v>0</v>
@@ -2690,18 +2874,18 @@
         <v>37</v>
       </c>
       <c r="J7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K7" t="s">
         <v>66</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="9" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>62</v>
@@ -2716,7 +2900,7 @@
     <row r="10" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="11" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>63</v>
@@ -2730,7 +2914,7 @@
     </row>
     <row r="13" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>64</v>
@@ -2752,10 +2936,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:H63"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2768,379 +2952,374 @@
     <col min="7" max="7" width="36.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>73</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>230</v>
-      </c>
+        <v>229</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>179</v>
+      <c r="A3" t="s">
+        <v>178</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D3" t="s">
-        <v>227</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="B4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C4" t="s">
-        <v>78</v>
-      </c>
-      <c r="D4" t="s">
-        <v>225</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>226</v>
-      </c>
+        <v>178</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>78</v>
+        <v>46</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>285</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>279</v>
-      </c>
+        <v>294</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>78</v>
+        <v>46</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>279</v>
-      </c>
+        <v>291</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>279</v>
+      <c r="E7" s="2"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="B9" t="s">
-        <v>63</v>
-      </c>
-      <c r="C9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
-        <v>222</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>224</v>
-      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B10" t="s">
         <v>63</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="B13" t="s">
-        <v>63</v>
-      </c>
-      <c r="C13" t="s">
-        <v>79</v>
-      </c>
-      <c r="D13" t="s">
-        <v>218</v>
-      </c>
-      <c r="E13" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="B14" t="s">
-        <v>63</v>
-      </c>
-      <c r="C14" t="s">
-        <v>79</v>
-      </c>
-      <c r="D14" t="s">
-        <v>219</v>
-      </c>
-      <c r="E14" t="s">
-        <v>221</v>
+        <v>178</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B16" t="s">
         <v>63</v>
       </c>
       <c r="C16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D16" t="s">
+        <v>249</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" t="s">
+        <v>80</v>
+      </c>
+      <c r="D17" t="s">
         <v>250</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E17" s="2" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="B17" t="s">
-        <v>63</v>
-      </c>
-      <c r="C17" t="s">
-        <v>81</v>
-      </c>
-      <c r="D17" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B18" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" t="s">
         <v>251</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="B18" t="s">
-        <v>63</v>
-      </c>
-      <c r="C18" t="s">
-        <v>81</v>
-      </c>
-      <c r="D18" t="s">
-        <v>252</v>
-      </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C20" t="s">
-        <v>79</v>
-      </c>
-      <c r="D20" t="s">
-        <v>200</v>
-      </c>
-      <c r="E20" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+        <v>178</v>
+      </c>
+      <c r="B20" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C21" t="s">
-        <v>79</v>
-      </c>
-      <c r="D21" t="s">
-        <v>189</v>
-      </c>
-      <c r="E21" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+        <v>178</v>
+      </c>
+      <c r="B21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>64</v>
+        <v>178</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C22" t="s">
-        <v>79</v>
-      </c>
-      <c r="D22" t="s">
-        <v>202</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="C22" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E22" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>64</v>
+        <v>178</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C23" t="s">
-        <v>79</v>
-      </c>
-      <c r="D23" t="s">
-        <v>203</v>
-      </c>
-      <c r="E23" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C24" t="s">
-        <v>79</v>
-      </c>
-      <c r="D24" t="s">
-        <v>204</v>
-      </c>
-      <c r="E24" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C23" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>64</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C25" t="s">
-        <v>79</v>
-      </c>
-      <c r="D25" t="s">
-        <v>205</v>
-      </c>
-      <c r="E25" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C26" t="s">
-        <v>79</v>
-      </c>
-      <c r="D26" t="s">
-        <v>206</v>
-      </c>
-      <c r="E26" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C25" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>64</v>
       </c>
@@ -3148,16 +3327,16 @@
         <v>63</v>
       </c>
       <c r="C27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D27" t="s">
-        <v>207</v>
-      </c>
-      <c r="E27" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>64</v>
       </c>
@@ -3165,16 +3344,16 @@
         <v>63</v>
       </c>
       <c r="C28" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D28" t="s">
-        <v>208</v>
-      </c>
-      <c r="E28" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>64</v>
       </c>
@@ -3182,14 +3361,348 @@
         <v>63</v>
       </c>
       <c r="C29" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D29" t="s">
+        <v>201</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" t="s">
+        <v>78</v>
+      </c>
+      <c r="D30" t="s">
+        <v>202</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C31" t="s">
+        <v>78</v>
+      </c>
+      <c r="D31" t="s">
+        <v>203</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32" t="s">
+        <v>78</v>
+      </c>
+      <c r="D32" t="s">
+        <v>204</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C33" t="s">
+        <v>78</v>
+      </c>
+      <c r="D33" t="s">
+        <v>205</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C34" t="s">
+        <v>78</v>
+      </c>
+      <c r="D34" t="s">
+        <v>206</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C35" t="s">
+        <v>78</v>
+      </c>
+      <c r="D35" t="s">
+        <v>207</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C36" t="s">
+        <v>78</v>
+      </c>
+      <c r="D36" t="s">
+        <v>208</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="E29" t="s">
-        <v>210</v>
-      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E37" s="2"/>
+    </row>
+    <row r="38" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H38" s="1"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D39" t="s">
+        <v>224</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="G40" s="1"/>
+    </row>
+    <row r="41" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="G41" s="1"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E42" s="2"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C43" t="s">
+        <v>40</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="H43" s="1"/>
+    </row>
+    <row r="44" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="H44" s="1"/>
+    </row>
+    <row r="45" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="H45" s="1"/>
+    </row>
+    <row r="46" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="H46" s="1"/>
+    </row>
+    <row r="47" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H47" s="1"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E48" s="2"/>
+    </row>
+    <row r="49" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E49" s="2"/>
+    </row>
+    <row r="50" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E50" s="2"/>
+    </row>
+    <row r="51" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E51" s="2"/>
+    </row>
+    <row r="52" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E52" s="2"/>
+    </row>
+    <row r="53" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E53" s="2"/>
+    </row>
+    <row r="54" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E54" s="2"/>
+    </row>
+    <row r="55" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E55" s="2"/>
+    </row>
+    <row r="56" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E56" s="2"/>
+    </row>
+    <row r="57" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E57" s="2"/>
+    </row>
+    <row r="58" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E58" s="2"/>
+    </row>
+    <row r="59" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E59" s="2"/>
+    </row>
+    <row r="60" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E60" s="2"/>
+    </row>
+    <row r="61" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E61" s="2"/>
+    </row>
+    <row r="62" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E62" s="2"/>
+    </row>
+    <row r="63" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E63" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -3213,40 +3726,40 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>232</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>236</v>
+      </c>
+      <c r="B3" t="s">
         <v>237</v>
-      </c>
-      <c r="B3" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.35"/>
@@ -3255,7 +3768,7 @@
         <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -3263,7 +3776,7 @@
         <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -3271,7 +3784,7 @@
         <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -3279,7 +3792,7 @@
         <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -3287,10 +3800,10 @@
         <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C11" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -3298,7 +3811,7 @@
         <v>37</v>
       </c>
       <c r="C13" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -3306,7 +3819,7 @@
         <v>37</v>
       </c>
       <c r="C14" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>
@@ -3331,19 +3844,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -3351,13 +3864,13 @@
         <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D3" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E3" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -3365,13 +3878,13 @@
         <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D4" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E4" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -3382,21 +3895,21 @@
         <v>50</v>
       </c>
       <c r="D6" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C8" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D8" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -3421,22 +3934,22 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>248</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -3444,13 +3957,13 @@
         <v>72</v>
       </c>
       <c r="B3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -3458,13 +3971,13 @@
         <v>72</v>
       </c>
       <c r="B5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -3472,10 +3985,10 @@
         <v>72</v>
       </c>
       <c r="B7" t="s">
+        <v>195</v>
+      </c>
+      <c r="E7" t="s">
         <v>196</v>
-      </c>
-      <c r="E7" t="s">
-        <v>197</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New test delivery for bact.
</commit_message>
<xml_diff>
--- a/test_data/resources/dwca_matrix_bacterioplankton.xlsx
+++ b/test_data/resources/dwca_matrix_bacterioplankton.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7920" tabRatio="687" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7920" tabRatio="687"/>
   </bookViews>
   <sheets>
     <sheet name="dwc_columns" sheetId="12" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="294">
   <si>
     <t>shark_sample_id_md5</t>
   </si>
@@ -284,9 +284,6 @@
     <t>sex_code</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
     <t>parentEventID</t>
   </si>
   <si>
@@ -410,9 +407,6 @@
     <t>measurementType</t>
   </si>
   <si>
-    <t># measurementTypeID</t>
-  </si>
-  <si>
     <t>measurementValue</t>
   </si>
   <si>
@@ -422,9 +416,6 @@
     <t>measurementUnit</t>
   </si>
   <si>
-    <t># measurementUnitID</t>
-  </si>
-  <si>
     <t>measurementAccuracy</t>
   </si>
   <si>
@@ -707,9 +698,6 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t># eventID</t>
-  </si>
-  <si>
     <t>comments</t>
   </si>
   <si>
@@ -806,30 +794,6 @@
     <t>from_value</t>
   </si>
   <si>
-    <t>TEST</t>
-  </si>
-  <si>
-    <t>SWEDEN</t>
-  </si>
-  <si>
-    <t>SLÄGGÖ</t>
-  </si>
-  <si>
-    <t>släggö</t>
-  </si>
-  <si>
-    <t>Å17</t>
-  </si>
-  <si>
-    <t>å17</t>
-  </si>
-  <si>
-    <t>test_source</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
     <t>visit_date</t>
   </si>
   <si>
@@ -924,6 +888,21 @@
   </si>
   <si>
     <t>analytical_laboratory_name_sv</t>
+  </si>
+  <si>
+    <t>eventID</t>
+  </si>
+  <si>
+    <t># id</t>
+  </si>
+  <si>
+    <t>measurementTypeID</t>
+  </si>
+  <si>
+    <t>measurementUnitID</t>
+  </si>
+  <si>
+    <t>present</t>
   </si>
 </sst>
 </file>
@@ -1275,8 +1254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1288,57 +1267,57 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>87</v>
-      </c>
-      <c r="B3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C3" t="s">
-        <v>87</v>
+        <v>290</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>228</v>
-      </c>
-      <c r="B4" t="s">
-        <v>228</v>
-      </c>
-      <c r="C4" t="s">
-        <v>228</v>
+        <v>289</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B6" t="s">
         <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1346,10 +1325,10 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1357,21 +1336,21 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C8" t="s">
-        <v>129</v>
+        <v>291</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1382,7 +1361,7 @@
         <v>79</v>
       </c>
       <c r="C10" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1393,7 +1372,7 @@
         <v>85</v>
       </c>
       <c r="C11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1404,26 +1383,26 @@
         <v>84</v>
       </c>
       <c r="C12" t="s">
-        <v>133</v>
+        <v>292</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C13" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C14" t="s">
         <v>38</v>
@@ -1434,7 +1413,7 @@
         <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C15" t="s">
         <v>40</v>
@@ -1442,10 +1421,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C16" t="s">
         <v>42</v>
@@ -1453,10 +1432,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C17" t="s">
         <v>44</v>
@@ -1464,18 +1443,18 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1483,7 +1462,7 @@
         <v>80</v>
       </c>
       <c r="B20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1491,7 +1470,7 @@
         <v>11</v>
       </c>
       <c r="B21" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1499,15 +1478,15 @@
         <v>13</v>
       </c>
       <c r="B22" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B23" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -1515,7 +1494,7 @@
         <v>47</v>
       </c>
       <c r="B24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -1523,7 +1502,7 @@
         <v>48</v>
       </c>
       <c r="B25" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -1531,7 +1510,7 @@
         <v>15</v>
       </c>
       <c r="B26" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1539,12 +1518,12 @@
         <v>17</v>
       </c>
       <c r="B27" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B28" t="s">
         <v>75</v>
@@ -1563,12 +1542,12 @@
         <v>21</v>
       </c>
       <c r="B30" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B31" t="s">
         <v>78</v>
@@ -1596,12 +1575,12 @@
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
@@ -1611,27 +1590,27 @@
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
@@ -1651,7 +1630,7 @@
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
@@ -1673,10 +1652,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I84"/>
+  <dimension ref="A1:I85"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C83" sqref="C83"/>
+    <sheetView topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1694,28 +1673,28 @@
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>73</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -1723,21 +1702,21 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B3" t="s">
         <v>62</v>
       </c>
       <c r="C3" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>270</v>
+        <v>258</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B4" t="s">
         <v>62</v>
@@ -1751,7 +1730,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B5" t="s">
         <v>62</v>
@@ -1765,32 +1744,32 @@
     </row>
     <row r="6" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>62</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>63</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1808,42 +1787,40 @@
       </c>
     </row>
     <row r="9" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>178</v>
-      </c>
-      <c r="B10" t="s">
-        <v>62</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="A9" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>175</v>
+      </c>
+      <c r="B11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>269</v>
-      </c>
       <c r="G11" s="2"/>
-      <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>62</v>
@@ -1852,698 +1829,699 @@
         <v>5</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>6</v>
+        <v>257</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>62</v>
       </c>
       <c r="C13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>178</v>
-      </c>
-      <c r="B14" t="s">
-        <v>62</v>
-      </c>
-      <c r="C14" t="s">
-        <v>19</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="G14" s="2"/>
-      <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B15" t="s">
         <v>62</v>
       </c>
       <c r="C15" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B16" t="s">
         <v>62</v>
       </c>
       <c r="C16" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F17" s="2"/>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>175</v>
+      </c>
+      <c r="B17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>178</v>
-      </c>
-      <c r="B18" t="s">
-        <v>62</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>175</v>
+      </c>
+      <c r="B19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" t="s">
         <v>11</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F19" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19"/>
-      <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>178</v>
-      </c>
-      <c r="B20" t="s">
-        <v>62</v>
-      </c>
-      <c r="C20" t="s">
+    <row r="20" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>175</v>
+      </c>
+      <c r="B21" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" t="s">
         <v>15</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F21" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G20" s="2"/>
-      <c r="H20" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>178</v>
-      </c>
-      <c r="B21" t="s">
-        <v>62</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="G21" s="2"/>
+      <c r="H21" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>175</v>
+      </c>
+      <c r="B22" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" t="s">
         <v>17</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F22" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="G21" s="2"/>
-      <c r="H21" s="3" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>178</v>
-      </c>
-      <c r="B22" t="s">
-        <v>62</v>
-      </c>
-      <c r="C22" t="s">
-        <v>21</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="3" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23"/>
-      <c r="F23" s="2"/>
+        <v>244</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>175</v>
+      </c>
+      <c r="B23" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" t="s">
+        <v>21</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="G23" s="2"/>
-    </row>
-    <row r="24" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C24" s="3" t="s">
+      <c r="H23" s="3" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+    </row>
+    <row r="25" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F24" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="G24" s="2"/>
-    </row>
-    <row r="25" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>106</v>
-      </c>
       <c r="F25" s="2" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F26" s="2"/>
+    <row r="26" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>252</v>
+      </c>
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>183</v>
-      </c>
-      <c r="B27" t="s">
-        <v>62</v>
-      </c>
-      <c r="D27" t="s">
+    <row r="27" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>180</v>
+      </c>
+      <c r="B28" t="s">
+        <v>62</v>
+      </c>
+      <c r="D28" t="s">
+        <v>152</v>
+      </c>
+      <c r="E28" t="s">
+        <v>169</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="G28" s="2"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>180</v>
+      </c>
+      <c r="B29" t="s">
+        <v>62</v>
+      </c>
+      <c r="D29" t="s">
+        <v>153</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="G29" s="2"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>180</v>
+      </c>
+      <c r="B30" t="s">
+        <v>62</v>
+      </c>
+      <c r="D30" t="s">
+        <v>154</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G30" s="2"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>180</v>
+      </c>
+      <c r="B31" t="s">
+        <v>62</v>
+      </c>
+      <c r="D31" t="s">
         <v>155</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F31" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="G31" s="2"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>180</v>
+      </c>
+      <c r="B32" t="s">
+        <v>62</v>
+      </c>
+      <c r="D32" t="s">
+        <v>156</v>
+      </c>
+      <c r="E32" t="s">
+        <v>170</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="G32" s="2"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>180</v>
+      </c>
+      <c r="B33" t="s">
+        <v>62</v>
+      </c>
+      <c r="D33" t="s">
+        <v>157</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G33" s="2"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>180</v>
+      </c>
+      <c r="B34" t="s">
+        <v>62</v>
+      </c>
+      <c r="D34" t="s">
+        <v>158</v>
+      </c>
+      <c r="E34" t="s">
+        <v>169</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G34" s="2"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>180</v>
+      </c>
+      <c r="B35" t="s">
+        <v>62</v>
+      </c>
+      <c r="D35" t="s">
+        <v>159</v>
+      </c>
+      <c r="E35" t="s">
+        <v>169</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G35" s="2"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>180</v>
+      </c>
+      <c r="B36" t="s">
+        <v>62</v>
+      </c>
+      <c r="D36" t="s">
+        <v>160</v>
+      </c>
+      <c r="E36" t="s">
+        <v>169</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G36" s="2"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>180</v>
+      </c>
+      <c r="B37" t="s">
+        <v>62</v>
+      </c>
+      <c r="D37" t="s">
+        <v>161</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="G37" s="2"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>180</v>
+      </c>
+      <c r="B38" t="s">
+        <v>62</v>
+      </c>
+      <c r="D38" t="s">
+        <v>162</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="G38" s="2"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>180</v>
+      </c>
+      <c r="B39" t="s">
+        <v>62</v>
+      </c>
+      <c r="D39" t="s">
+        <v>163</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="G39" s="2"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>180</v>
+      </c>
+      <c r="B40" t="s">
+        <v>62</v>
+      </c>
+      <c r="D40" t="s">
+        <v>164</v>
+      </c>
+      <c r="E40" t="s">
+        <v>171</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="G40" s="2"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>180</v>
+      </c>
+      <c r="B41" t="s">
+        <v>62</v>
+      </c>
+      <c r="D41" t="s">
+        <v>165</v>
+      </c>
+      <c r="E41" t="s">
+        <v>171</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="G41" s="2"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>180</v>
+      </c>
+      <c r="B42" t="s">
+        <v>62</v>
+      </c>
+      <c r="D42" t="s">
+        <v>166</v>
+      </c>
+      <c r="E42" t="s">
         <v>172</v>
       </c>
-      <c r="F27" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="G27" s="2"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>183</v>
-      </c>
-      <c r="B28" t="s">
-        <v>62</v>
-      </c>
-      <c r="D28" t="s">
-        <v>156</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="G28" s="2"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>183</v>
-      </c>
-      <c r="B29" t="s">
-        <v>62</v>
-      </c>
-      <c r="D29" t="s">
-        <v>157</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="G29" s="2"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>183</v>
-      </c>
-      <c r="B30" t="s">
-        <v>62</v>
-      </c>
-      <c r="D30" t="s">
-        <v>158</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="G30" s="2"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>183</v>
-      </c>
-      <c r="B31" t="s">
-        <v>62</v>
-      </c>
-      <c r="D31" t="s">
-        <v>159</v>
-      </c>
-      <c r="E31" t="s">
-        <v>173</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="G31" s="2"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>183</v>
-      </c>
-      <c r="B32" t="s">
-        <v>62</v>
-      </c>
-      <c r="D32" t="s">
-        <v>160</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="G32" s="2"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>183</v>
-      </c>
-      <c r="B33" t="s">
-        <v>62</v>
-      </c>
-      <c r="D33" t="s">
-        <v>161</v>
-      </c>
-      <c r="E33" t="s">
-        <v>172</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="G33" s="2"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>183</v>
-      </c>
-      <c r="B34" t="s">
-        <v>62</v>
-      </c>
-      <c r="D34" t="s">
-        <v>162</v>
-      </c>
-      <c r="E34" t="s">
-        <v>172</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="G34" s="2"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>183</v>
-      </c>
-      <c r="B35" t="s">
-        <v>62</v>
-      </c>
-      <c r="D35" t="s">
-        <v>163</v>
-      </c>
-      <c r="E35" t="s">
-        <v>172</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="G35" s="2"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>183</v>
-      </c>
-      <c r="B36" t="s">
-        <v>62</v>
-      </c>
-      <c r="D36" t="s">
-        <v>164</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="G36" s="2"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>183</v>
-      </c>
-      <c r="B37" t="s">
-        <v>62</v>
-      </c>
-      <c r="D37" t="s">
-        <v>165</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="G37" s="2"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>183</v>
-      </c>
-      <c r="B38" t="s">
-        <v>62</v>
-      </c>
-      <c r="D38" t="s">
-        <v>166</v>
-      </c>
-      <c r="F38" s="2" t="s">
+      <c r="F42" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="G38" s="2"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>183</v>
-      </c>
-      <c r="B39" t="s">
-        <v>62</v>
-      </c>
-      <c r="D39" t="s">
+      <c r="G42" s="2"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>180</v>
+      </c>
+      <c r="B43" t="s">
+        <v>62</v>
+      </c>
+      <c r="D43" t="s">
         <v>167</v>
       </c>
-      <c r="E39" t="s">
-        <v>174</v>
-      </c>
-      <c r="F39" s="2" t="s">
+      <c r="F43" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="G39" s="2"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>183</v>
-      </c>
-      <c r="B40" t="s">
-        <v>62</v>
-      </c>
-      <c r="D40" t="s">
+      <c r="G43" s="2"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>180</v>
+      </c>
+      <c r="B44" t="s">
+        <v>62</v>
+      </c>
+      <c r="D44" t="s">
         <v>168</v>
       </c>
-      <c r="E40" t="s">
-        <v>174</v>
-      </c>
-      <c r="F40" s="2" t="s">
+      <c r="F44" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="G40" s="2"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>183</v>
-      </c>
-      <c r="B41" t="s">
-        <v>62</v>
-      </c>
-      <c r="D41" t="s">
-        <v>169</v>
-      </c>
-      <c r="E41" t="s">
-        <v>175</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="G41" s="2"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>183</v>
-      </c>
-      <c r="B42" t="s">
-        <v>62</v>
-      </c>
-      <c r="D42" t="s">
-        <v>170</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="G42" s="2"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>183</v>
-      </c>
-      <c r="B43" t="s">
-        <v>62</v>
-      </c>
-      <c r="D43" t="s">
-        <v>171</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="G43" s="2"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F44" s="2"/>
       <c r="G44" s="2"/>
     </row>
-    <row r="45" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C45" s="3" t="s">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+    </row>
+    <row r="46" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C46" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F45" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="G45" s="2"/>
-    </row>
-    <row r="46" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>106</v>
-      </c>
       <c r="F46" s="2" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="G46" s="2"/>
     </row>
-    <row r="47" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="3"/>
-      <c r="F47" s="2"/>
+    <row r="47" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>252</v>
+      </c>
       <c r="G47" s="2"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>178</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C48" t="s">
+    <row r="48" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="3"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>175</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C49" t="s">
         <v>5</v>
       </c>
-      <c r="F48" s="2" t="s">
+      <c r="F49" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="G48" s="2"/>
-      <c r="H48" s="1"/>
-    </row>
-    <row r="49" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>269</v>
       </c>
       <c r="G49" s="2"/>
       <c r="H49" s="1"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>178</v>
+    <row r="50" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C50" t="s">
-        <v>7</v>
+      <c r="C50" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>8</v>
+        <v>257</v>
       </c>
       <c r="G50" s="2"/>
+      <c r="H50" s="1"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>178</v>
-      </c>
-      <c r="B51" t="s">
+        <v>175</v>
+      </c>
+      <c r="B51" s="3" t="s">
         <v>63</v>
       </c>
       <c r="C51" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="G51" s="2"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B52" t="s">
         <v>63</v>
       </c>
       <c r="C52" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="G52" s="2"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B53" t="s">
         <v>63</v>
       </c>
       <c r="C53" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G53" s="2"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B54" t="s">
         <v>63</v>
       </c>
       <c r="C54" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="G54" s="2"/>
-      <c r="H54" s="3"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B55" t="s">
         <v>63</v>
       </c>
       <c r="C55" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G55" s="2"/>
       <c r="H55" s="3"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B56" t="s">
         <v>63</v>
       </c>
       <c r="C56" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="G56" s="2"/>
+      <c r="H56" s="3"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B57" t="s">
         <v>63</v>
       </c>
       <c r="C57" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G57" s="2"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B58" t="s">
         <v>63</v>
       </c>
       <c r="C58" t="s">
+        <v>3</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G58" s="2"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>175</v>
+      </c>
+      <c r="B59" t="s">
+        <v>63</v>
+      </c>
+      <c r="C59" t="s">
         <v>13</v>
       </c>
-      <c r="F58" s="2" t="s">
+      <c r="F59" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="G58" s="2"/>
-    </row>
-    <row r="59" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F59" s="2" t="s">
-        <v>280</v>
       </c>
       <c r="G59" s="2"/>
     </row>
     <row r="60" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>63</v>
@@ -2552,29 +2530,29 @@
         <v>33</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>295</v>
+        <v>268</v>
       </c>
       <c r="G60" s="2"/>
     </row>
     <row r="61" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="3"/>
-      <c r="E61" s="3"/>
-      <c r="F61" s="2"/>
+      <c r="A61" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>283</v>
+      </c>
       <c r="G61" s="2"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>64</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C62" t="s">
-        <v>36</v>
-      </c>
-      <c r="F62" s="2" t="s">
-        <v>37</v>
-      </c>
+    <row r="62" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="3"/>
+      <c r="E62" s="3"/>
+      <c r="F62" s="2"/>
       <c r="G62" s="2"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
@@ -2585,10 +2563,10 @@
         <v>63</v>
       </c>
       <c r="C63" t="s">
-        <v>85</v>
+        <v>36</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
       <c r="G63" s="2"/>
     </row>
@@ -2600,81 +2578,93 @@
         <v>63</v>
       </c>
       <c r="C64" t="s">
+        <v>85</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G64" s="2"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>64</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C65" t="s">
         <v>84</v>
       </c>
-      <c r="F64" s="2" t="s">
+      <c r="F65" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="G64" s="2"/>
-    </row>
-    <row r="65" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F65" s="2"/>
       <c r="G65" s="2"/>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>183</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D66" t="s">
-        <v>188</v>
-      </c>
-      <c r="E66" t="s">
-        <v>187</v>
-      </c>
-      <c r="F66" s="2" t="s">
-        <v>176</v>
-      </c>
+    <row r="66" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F66" s="2"/>
       <c r="G66" s="2"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C67" t="s">
-        <v>38</v>
+      <c r="D67" t="s">
+        <v>185</v>
+      </c>
+      <c r="E67" t="s">
+        <v>184</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>39</v>
+        <v>173</v>
       </c>
       <c r="G67" s="2"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C68" s="3" t="s">
+      <c r="C68" t="s">
+        <v>38</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G68" s="2"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>180</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C69" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="F68" s="2" t="s">
+      <c r="F69" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G68" s="2"/>
-    </row>
-    <row r="69" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G69" s="2"/>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G70" s="2"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G71" s="2"/>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>227</v>
-      </c>
       <c r="G72" s="2"/>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>224</v>
+      </c>
       <c r="G73" s="2"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -2709,6 +2699,9 @@
     </row>
     <row r="84" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G84" s="2"/>
+    </row>
+    <row r="85" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G85" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -2721,7 +2714,7 @@
   <dimension ref="A1:Q13"/>
   <sheetViews>
     <sheetView topLeftCell="E1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I38" sqref="I38"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2745,19 +2738,19 @@
   <sheetData>
     <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>83</v>
@@ -2793,12 +2786,12 @@
         <v>61</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B3" t="s">
         <v>62</v>
@@ -2821,7 +2814,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B5" t="s">
         <v>63</v>
@@ -2880,12 +2873,12 @@
         <v>66</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="9" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>62</v>
@@ -2900,7 +2893,7 @@
     <row r="10" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="11" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>63</v>
@@ -2914,7 +2907,7 @@
     </row>
     <row r="13" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>64</v>
@@ -2938,7 +2931,7 @@
   </sheetPr>
   <dimension ref="A1:H63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
@@ -2954,10 +2947,10 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>81</v>
@@ -2966,13 +2959,13 @@
         <v>82</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>73</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2982,7 +2975,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B3" t="s">
         <v>62</v>
@@ -2991,7 +2984,7 @@
         <v>46</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>35</v>
@@ -3000,7 +2993,7 @@
     </row>
     <row r="4" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>62</v>
@@ -3009,16 +3002,16 @@
         <v>46</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>294</v>
+        <v>282</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>296</v>
+        <v>284</v>
       </c>
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>62</v>
@@ -3027,16 +3020,16 @@
         <v>46</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>294</v>
+        <v>282</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>297</v>
+        <v>285</v>
       </c>
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>62</v>
@@ -3045,10 +3038,10 @@
         <v>46</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>291</v>
+        <v>279</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>292</v>
+        <v>280</v>
       </c>
       <c r="G6" s="1"/>
     </row>
@@ -3058,7 +3051,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B8" t="s">
         <v>63</v>
@@ -3067,7 +3060,7 @@
         <v>77</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>4</v>
@@ -3080,7 +3073,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B10" t="s">
         <v>63</v>
@@ -3089,7 +3082,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>2</v>
@@ -3097,7 +3090,7 @@
     </row>
     <row r="11" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>63</v>
@@ -3106,16 +3099,16 @@
         <v>1</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B12" t="s">
         <v>63</v>
@@ -3124,10 +3117,10 @@
         <v>1</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -3137,7 +3130,7 @@
     </row>
     <row r="14" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>63</v>
@@ -3146,15 +3139,15 @@
         <v>80</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>278</v>
+        <v>266</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
     </row>
     <row r="15" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>63</v>
@@ -3163,7 +3156,7 @@
         <v>80</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>279</v>
+        <v>267</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>10</v>
@@ -3171,7 +3164,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B16" t="s">
         <v>63</v>
@@ -3180,15 +3173,15 @@
         <v>80</v>
       </c>
       <c r="D16" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B17" t="s">
         <v>63</v>
@@ -3197,15 +3190,15 @@
         <v>80</v>
       </c>
       <c r="D17" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B18" t="s">
         <v>63</v>
@@ -3214,7 +3207,7 @@
         <v>80</v>
       </c>
       <c r="D18" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>65</v>
@@ -3225,7 +3218,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B20" t="s">
         <v>63</v>
@@ -3234,15 +3227,15 @@
         <v>78</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>283</v>
+        <v>271</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>281</v>
+        <v>269</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B21" t="s">
         <v>63</v>
@@ -3251,15 +3244,15 @@
         <v>78</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>282</v>
+        <v>270</v>
       </c>
     </row>
     <row r="22" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>63</v>
@@ -3268,15 +3261,15 @@
         <v>78</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="23" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>63</v>
@@ -3285,10 +3278,10 @@
         <v>78</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="24" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -3304,13 +3297,13 @@
         <v>63</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>293</v>
+        <v>281</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
       <c r="G25" s="1"/>
     </row>
@@ -3330,10 +3323,10 @@
         <v>78</v>
       </c>
       <c r="D27" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -3347,10 +3340,10 @@
         <v>78</v>
       </c>
       <c r="D28" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -3364,10 +3357,10 @@
         <v>78</v>
       </c>
       <c r="D29" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -3381,10 +3374,10 @@
         <v>78</v>
       </c>
       <c r="D30" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -3398,10 +3391,10 @@
         <v>78</v>
       </c>
       <c r="D31" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -3415,10 +3408,10 @@
         <v>78</v>
       </c>
       <c r="D32" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -3432,10 +3425,10 @@
         <v>78</v>
       </c>
       <c r="D33" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -3449,10 +3442,10 @@
         <v>78</v>
       </c>
       <c r="D34" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -3466,10 +3459,10 @@
         <v>78</v>
       </c>
       <c r="D35" t="s">
+        <v>204</v>
+      </c>
+      <c r="E35" s="2" t="s">
         <v>207</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -3483,10 +3476,10 @@
         <v>78</v>
       </c>
       <c r="D36" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -3494,7 +3487,7 @@
     </row>
     <row r="38" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>64</v>
@@ -3503,7 +3496,7 @@
         <v>42</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>276</v>
+        <v>264</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>43</v>
@@ -3512,7 +3505,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>64</v>
@@ -3521,15 +3514,15 @@
         <v>42</v>
       </c>
       <c r="D39" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="40" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>64</v>
@@ -3538,16 +3531,16 @@
         <v>42</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>271</v>
+        <v>259</v>
       </c>
       <c r="G40" s="1"/>
     </row>
     <row r="41" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>64</v>
@@ -3556,10 +3549,10 @@
         <v>42</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
       <c r="G41" s="1"/>
     </row>
@@ -3568,7 +3561,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>64</v>
@@ -3577,16 +3570,16 @@
         <v>40</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>287</v>
+        <v>275</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>285</v>
+        <v>273</v>
       </c>
       <c r="H43" s="1"/>
     </row>
     <row r="44" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>64</v>
@@ -3595,16 +3588,16 @@
         <v>40</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>298</v>
+        <v>286</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>300</v>
+        <v>288</v>
       </c>
       <c r="H44" s="1"/>
     </row>
     <row r="45" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>64</v>
@@ -3613,16 +3606,16 @@
         <v>40</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>298</v>
+        <v>286</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>299</v>
+        <v>287</v>
       </c>
       <c r="H45" s="1"/>
     </row>
     <row r="46" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>64</v>
@@ -3631,16 +3624,16 @@
         <v>40</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>288</v>
+        <v>276</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>286</v>
+        <v>274</v>
       </c>
       <c r="H46" s="1"/>
     </row>
     <row r="47" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>64</v>
@@ -3649,7 +3642,7 @@
         <v>40</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>289</v>
+        <v>277</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>41</v>
@@ -3726,40 +3719,40 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B3" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.35"/>
@@ -3768,7 +3761,7 @@
         <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -3776,7 +3769,7 @@
         <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -3784,7 +3777,7 @@
         <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -3792,7 +3785,7 @@
         <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -3800,10 +3793,10 @@
         <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C11" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -3811,7 +3804,7 @@
         <v>37</v>
       </c>
       <c r="C13" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -3819,7 +3812,7 @@
         <v>37</v>
       </c>
       <c r="C14" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -3829,10 +3822,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3844,72 +3837,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" t="s">
-        <v>263</v>
-      </c>
-      <c r="D3" t="s">
-        <v>264</v>
-      </c>
-      <c r="E3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" t="s">
-        <v>265</v>
-      </c>
-      <c r="D4" t="s">
-        <v>266</v>
-      </c>
-      <c r="E4" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D6" t="s">
-        <v>262</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>267</v>
-      </c>
-      <c r="C8" t="s">
-        <v>268</v>
-      </c>
-      <c r="D8" t="s">
-        <v>268</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -3934,22 +3874,22 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>247</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -3957,13 +3897,13 @@
         <v>72</v>
       </c>
       <c r="B3" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C3" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D3" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -3971,13 +3911,13 @@
         <v>72</v>
       </c>
       <c r="B5" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C5" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D5" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -3985,10 +3925,10 @@
         <v>72</v>
       </c>
       <c r="B7" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E7" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Excel updated for bacterioplankton.
</commit_message>
<xml_diff>
--- a/test_data/resources/dwca_matrix_bacterioplankton.xlsx
+++ b/test_data/resources/dwca_matrix_bacterioplankton.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7920" tabRatio="687"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7920" tabRatio="687" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="dwc_columns" sheetId="12" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="286">
   <si>
     <t>shark_sample_id_md5</t>
   </si>
@@ -707,33 +707,6 @@
     <t>exclude_value</t>
   </si>
   <si>
-    <t># SLÄGGÖ</t>
-  </si>
-  <si>
-    <t># N14 FALKENBERG</t>
-  </si>
-  <si>
-    <t># ANHOLT E</t>
-  </si>
-  <si>
-    <t># TOR20</t>
-  </si>
-  <si>
-    <t>delivery_datatype</t>
-  </si>
-  <si>
-    <t># Phytoplankton</t>
-  </si>
-  <si>
-    <t># Zoobenthos</t>
-  </si>
-  <si>
-    <t># Zooplankton</t>
-  </si>
-  <si>
-    <t># ABCD</t>
-  </si>
-  <si>
     <t>Flagellates</t>
   </si>
   <si>
@@ -827,9 +800,6 @@
     <t>VisitYear</t>
   </si>
   <si>
-    <t>sample_orderer_code</t>
-  </si>
-  <si>
     <t>sample_project_code</t>
   </si>
   <si>
@@ -872,9 +842,6 @@
     <t>SamplingLaboratoryName</t>
   </si>
   <si>
-    <t>delivery_orderer_code</t>
-  </si>
-  <si>
     <t>sampling_laboratory_name_sv</t>
   </si>
   <si>
@@ -903,6 +870,15 @@
   </si>
   <si>
     <t>present</t>
+  </si>
+  <si>
+    <t>SHARK - Marine bacterioplankton monitoring in Sweden since 1989</t>
+  </si>
+  <si>
+    <t>Swedish Agency for Marine and Water Management</t>
+  </si>
+  <si>
+    <t>Swedish Meteorological and Hydrological Institute</t>
   </si>
 </sst>
 </file>
@@ -1252,10 +1228,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C53"/>
+  <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1278,24 +1254,24 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1339,7 +1315,7 @@
         <v>109</v>
       </c>
       <c r="C8" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1383,7 +1359,7 @@
         <v>84</v>
       </c>
       <c r="C12" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1614,32 +1590,37 @@
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="A44" s="3" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>32</v>
+        <v>191</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>106</v>
+        <v>33</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="2"/>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1654,8 +1635,8 @@
   </sheetPr>
   <dimension ref="A1:I85"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F51" sqref="F51"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1671,12 +1652,12 @@
     <col min="9" max="9" width="35.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>174</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>49</v>
@@ -1697,265 +1678,260 @@
         <v>225</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>175</v>
-      </c>
-      <c r="B3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C3" t="s">
+    <row r="3" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>175</v>
+      </c>
+      <c r="B9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" t="s">
         <v>191</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>175</v>
-      </c>
-      <c r="B4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="F9" t="s">
+        <v>242</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>175</v>
+      </c>
+      <c r="B11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" t="s">
         <v>47</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G11" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>175</v>
-      </c>
-      <c r="B5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C5" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>175</v>
+      </c>
+      <c r="B12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" t="s">
         <v>48</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G12" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C6" s="3" t="s">
+    <row r="13" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="F13" s="2"/>
+      <c r="G13" s="2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="F14" s="2"/>
+      <c r="G14" s="2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>64</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="B15" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" t="s">
         <v>75</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G15" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+    <row r="16" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="B16" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>175</v>
-      </c>
-      <c r="B11" t="s">
-        <v>62</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="G16" s="2" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>175</v>
+      </c>
+      <c r="B18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F18" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C12" s="3" t="s">
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="G12" s="2"/>
-      <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C13" s="3" t="s">
+      <c r="F19" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="G19" s="2"/>
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F20" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="2"/>
-      <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C14" s="3" t="s">
+      <c r="G20" s="2"/>
+      <c r="H20" s="1"/>
+    </row>
+    <row r="21" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F21" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>175</v>
-      </c>
-      <c r="B15" t="s">
-        <v>62</v>
-      </c>
-      <c r="C15" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G15" s="2"/>
-      <c r="H15" s="1"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>175</v>
-      </c>
-      <c r="B16" t="s">
-        <v>62</v>
-      </c>
-      <c r="C16" t="s">
-        <v>27</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G16" s="2"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>175</v>
-      </c>
-      <c r="B17" t="s">
-        <v>62</v>
-      </c>
-      <c r="C17" t="s">
-        <v>29</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G17" s="2"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>175</v>
-      </c>
-      <c r="B19" t="s">
-        <v>62</v>
-      </c>
-      <c r="C19" t="s">
-        <v>11</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>175</v>
-      </c>
-      <c r="B21" t="s">
-        <v>62</v>
-      </c>
-      <c r="C21" t="s">
-        <v>15</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="G21" s="2"/>
-      <c r="H21" t="s">
-        <v>244</v>
-      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -1965,15 +1941,13 @@
         <v>62</v>
       </c>
       <c r="C22" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G22" s="2"/>
-      <c r="H22" s="3" t="s">
-        <v>244</v>
-      </c>
+      <c r="H22" s="1"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -1983,116 +1957,113 @@
         <v>62</v>
       </c>
       <c r="C23" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G23" s="2"/>
-      <c r="H23" s="3" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24"/>
-      <c r="F24" s="2"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>175</v>
+      </c>
+      <c r="B24" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" t="s">
+        <v>29</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="G24" s="2"/>
-    </row>
-    <row r="25" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>251</v>
-      </c>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F25" s="2"/>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>105</v>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>175</v>
+      </c>
+      <c r="B26" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26" t="s">
+        <v>11</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>252</v>
+        <v>12</v>
       </c>
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B28" t="s">
         <v>62</v>
       </c>
-      <c r="D28" t="s">
-        <v>152</v>
-      </c>
-      <c r="E28" t="s">
-        <v>169</v>
+      <c r="C28" t="s">
+        <v>15</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>135</v>
+        <v>16</v>
       </c>
       <c r="G28" s="2"/>
+      <c r="H28" t="s">
+        <v>235</v>
+      </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B29" t="s">
         <v>62</v>
       </c>
-      <c r="D29" t="s">
-        <v>153</v>
+      <c r="C29" t="s">
+        <v>17</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>136</v>
+        <v>18</v>
       </c>
       <c r="G29" s="2"/>
+      <c r="H29" s="3" t="s">
+        <v>235</v>
+      </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B30" t="s">
         <v>62</v>
       </c>
-      <c r="D30" t="s">
-        <v>154</v>
+      <c r="C30" t="s">
+        <v>21</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>137</v>
+        <v>22</v>
       </c>
       <c r="G30" s="2"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>180</v>
-      </c>
-      <c r="B31" t="s">
-        <v>62</v>
-      </c>
-      <c r="D31" t="s">
-        <v>155</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>138</v>
-      </c>
+      <c r="H30" s="3" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31"/>
+      <c r="F31" s="2"/>
       <c r="G31" s="2"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -2103,13 +2074,13 @@
         <v>62</v>
       </c>
       <c r="D32" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E32" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="G32" s="2"/>
     </row>
@@ -2121,10 +2092,10 @@
         <v>62</v>
       </c>
       <c r="D33" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="G33" s="2"/>
     </row>
@@ -2136,13 +2107,10 @@
         <v>62</v>
       </c>
       <c r="D34" t="s">
-        <v>158</v>
-      </c>
-      <c r="E34" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="G34" s="2"/>
     </row>
@@ -2154,13 +2122,10 @@
         <v>62</v>
       </c>
       <c r="D35" t="s">
-        <v>159</v>
-      </c>
-      <c r="E35" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="G35" s="2"/>
     </row>
@@ -2172,13 +2137,13 @@
         <v>62</v>
       </c>
       <c r="D36" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="E36" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G36" s="2"/>
     </row>
@@ -2190,10 +2155,10 @@
         <v>62</v>
       </c>
       <c r="D37" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="G37" s="2"/>
     </row>
@@ -2205,10 +2170,13 @@
         <v>62</v>
       </c>
       <c r="D38" t="s">
-        <v>162</v>
+        <v>158</v>
+      </c>
+      <c r="E38" t="s">
+        <v>169</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="G38" s="2"/>
     </row>
@@ -2220,10 +2188,13 @@
         <v>62</v>
       </c>
       <c r="D39" t="s">
-        <v>163</v>
+        <v>159</v>
+      </c>
+      <c r="E39" t="s">
+        <v>169</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="G39" s="2"/>
     </row>
@@ -2235,13 +2206,13 @@
         <v>62</v>
       </c>
       <c r="D40" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="E40" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="G40" s="2"/>
     </row>
@@ -2253,13 +2224,10 @@
         <v>62</v>
       </c>
       <c r="D41" t="s">
-        <v>165</v>
-      </c>
-      <c r="E41" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="G41" s="2"/>
     </row>
@@ -2271,13 +2239,10 @@
         <v>62</v>
       </c>
       <c r="D42" t="s">
-        <v>166</v>
-      </c>
-      <c r="E42" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="G42" s="2"/>
     </row>
@@ -2289,10 +2254,10 @@
         <v>62</v>
       </c>
       <c r="D43" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="G43" s="2"/>
     </row>
@@ -2304,83 +2269,90 @@
         <v>62</v>
       </c>
       <c r="D44" t="s">
+        <v>164</v>
+      </c>
+      <c r="E44" t="s">
+        <v>171</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="G44" s="2"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>180</v>
+      </c>
+      <c r="B45" t="s">
+        <v>62</v>
+      </c>
+      <c r="D45" t="s">
+        <v>165</v>
+      </c>
+      <c r="E45" t="s">
+        <v>171</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="G45" s="2"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>180</v>
+      </c>
+      <c r="B46" t="s">
+        <v>62</v>
+      </c>
+      <c r="D46" t="s">
+        <v>166</v>
+      </c>
+      <c r="E46" t="s">
+        <v>172</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="G46" s="2"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>180</v>
+      </c>
+      <c r="B47" t="s">
+        <v>62</v>
+      </c>
+      <c r="D47" t="s">
+        <v>167</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G47" s="2"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>180</v>
+      </c>
+      <c r="B48" t="s">
+        <v>62</v>
+      </c>
+      <c r="D48" t="s">
         <v>168</v>
       </c>
-      <c r="F44" s="2" t="s">
+      <c r="F48" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="G44" s="2"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F45" s="2"/>
-      <c r="G45" s="2"/>
-    </row>
-    <row r="46" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="G46" s="2"/>
-    </row>
-    <row r="47" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="G47" s="2"/>
-    </row>
-    <row r="48" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="3"/>
-      <c r="F48" s="2"/>
       <c r="G48" s="2"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>175</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C49" t="s">
-        <v>5</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="F49" s="2"/>
       <c r="G49" s="2"/>
-      <c r="H49" s="1"/>
-    </row>
-    <row r="50" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>257</v>
-      </c>
+    </row>
+    <row r="50" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="3"/>
+      <c r="F50" s="2"/>
       <c r="G50" s="2"/>
-      <c r="H50" s="1"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
@@ -2390,40 +2362,42 @@
         <v>63</v>
       </c>
       <c r="C51" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G51" s="2"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>175</v>
-      </c>
-      <c r="B52" t="s">
-        <v>63</v>
-      </c>
-      <c r="C52" t="s">
-        <v>19</v>
+      <c r="H51" s="1"/>
+    </row>
+    <row r="52" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>20</v>
+        <v>248</v>
       </c>
       <c r="G52" s="2"/>
+      <c r="H52" s="1"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>175</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="3" t="s">
         <v>63</v>
       </c>
       <c r="C53" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="G53" s="2"/>
     </row>
@@ -2435,10 +2409,10 @@
         <v>63</v>
       </c>
       <c r="C54" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="G54" s="2"/>
     </row>
@@ -2450,13 +2424,12 @@
         <v>63</v>
       </c>
       <c r="C55" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="G55" s="2"/>
-      <c r="H55" s="3"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
@@ -2466,13 +2439,12 @@
         <v>63</v>
       </c>
       <c r="C56" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="G56" s="2"/>
-      <c r="H56" s="3"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
@@ -2482,12 +2454,13 @@
         <v>63</v>
       </c>
       <c r="C57" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="G57" s="2"/>
+      <c r="H57" s="3"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
@@ -2497,12 +2470,13 @@
         <v>63</v>
       </c>
       <c r="C58" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="G58" s="2"/>
+      <c r="H58" s="3"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
@@ -2512,40 +2486,40 @@
         <v>63</v>
       </c>
       <c r="C59" t="s">
+        <v>1</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G59" s="2"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>175</v>
+      </c>
+      <c r="B60" t="s">
+        <v>63</v>
+      </c>
+      <c r="C60" t="s">
+        <v>3</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G60" s="2"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>175</v>
+      </c>
+      <c r="B61" t="s">
+        <v>63</v>
+      </c>
+      <c r="C61" t="s">
         <v>13</v>
       </c>
-      <c r="F59" s="2" t="s">
+      <c r="F61" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="G59" s="2"/>
-    </row>
-    <row r="60" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F60" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="G60" s="2"/>
-    </row>
-    <row r="61" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F61" s="2" t="s">
-        <v>283</v>
       </c>
       <c r="G61" s="2"/>
     </row>
@@ -2713,7 +2687,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q13"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
@@ -2741,7 +2715,7 @@
         <v>174</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>176</v>
@@ -2750,7 +2724,7 @@
         <v>182</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>83</v>
@@ -2931,14 +2905,15 @@
   </sheetPr>
   <dimension ref="A1:H63"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.28515625" style="3" customWidth="1"/>
-    <col min="2" max="3" width="24.28515625" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" customWidth="1"/>
+    <col min="3" max="3" width="36.42578125" customWidth="1"/>
     <col min="4" max="4" width="28.42578125" customWidth="1"/>
     <col min="5" max="5" width="26.140625" customWidth="1"/>
     <col min="6" max="6" width="32" customWidth="1"/>
@@ -2950,7 +2925,7 @@
         <v>174</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>81</v>
@@ -2980,16 +2955,18 @@
       <c r="B3" t="s">
         <v>62</v>
       </c>
-      <c r="C3" t="s">
-        <v>46</v>
+      <c r="C3" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="1"/>
+      <c r="G3" s="3" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="4" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -2998,14 +2975,14 @@
       <c r="B4" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>46</v>
+      <c r="C4" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
       <c r="G4" s="1"/>
     </row>
@@ -3016,14 +2993,14 @@
       <c r="B5" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>46</v>
+      <c r="C5" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
       <c r="G5" s="1"/>
     </row>
@@ -3034,99 +3011,110 @@
       <c r="B6" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>46</v>
+      <c r="C6" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E7" s="2"/>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="B8" t="s">
-        <v>63</v>
+      <c r="B8" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E10" s="2"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="B10" t="s">
-        <v>63</v>
-      </c>
-      <c r="C10" s="2" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="B12" t="s">
-        <v>63</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
@@ -3136,85 +3124,88 @@
         <v>63</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C15" s="2" t="s">
+      <c r="D17" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="E15" s="2" t="s">
+      <c r="D18" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="B16" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B19" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" t="s">
         <v>80</v>
       </c>
-      <c r="D16" t="s">
-        <v>245</v>
-      </c>
-      <c r="E16" s="2" t="s">
+      <c r="D19" t="s">
+        <v>236</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="B17" t="s">
-        <v>63</v>
-      </c>
-      <c r="C17" t="s">
-        <v>80</v>
-      </c>
-      <c r="D17" t="s">
-        <v>246</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="B18" t="s">
-        <v>63</v>
-      </c>
-      <c r="C18" t="s">
-        <v>80</v>
-      </c>
-      <c r="D18" t="s">
-        <v>247</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
@@ -3223,14 +3214,14 @@
       <c r="B20" t="s">
         <v>63</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>271</v>
+      <c r="C20" t="s">
+        <v>80</v>
+      </c>
+      <c r="D20" t="s">
+        <v>237</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>269</v>
+        <v>195</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -3240,48 +3231,34 @@
       <c r="B21" t="s">
         <v>63</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>272</v>
+      <c r="C21" t="s">
+        <v>80</v>
+      </c>
+      <c r="D21" t="s">
+        <v>238</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" t="s">
         <v>63</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>215</v>
+      <c r="D23" s="3" t="s">
+        <v>261</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>217</v>
+        <v>259</v>
       </c>
     </row>
     <row r="24" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -3300,10 +3277,10 @@
         <v>115</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="G25" s="1"/>
     </row>
@@ -3496,7 +3473,7 @@
         <v>42</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>43</v>
@@ -3531,10 +3508,10 @@
         <v>42</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="G40" s="1"/>
     </row>
@@ -3549,10 +3526,10 @@
         <v>42</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="G41" s="1"/>
     </row>
@@ -3570,10 +3547,10 @@
         <v>40</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
       <c r="H43" s="1"/>
     </row>
@@ -3588,10 +3565,10 @@
         <v>40</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>288</v>
+        <v>277</v>
       </c>
       <c r="H44" s="1"/>
     </row>
@@ -3606,10 +3583,10 @@
         <v>40</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
       <c r="H45" s="1"/>
     </row>
@@ -3624,10 +3601,10 @@
         <v>40</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="H46" s="1"/>
     </row>
@@ -3642,7 +3619,7 @@
         <v>40</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>41</v>
@@ -3705,10 +3682,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3733,86 +3710,18 @@
     </row>
     <row r="3" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>232</v>
-      </c>
-      <c r="B3" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+      <c r="C3" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" t="s">
         <v>229</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" t="s">
-        <v>228</v>
-      </c>
-      <c r="C11" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" t="s">
-        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -3824,8 +3733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3843,10 +3752,10 @@
         <v>49</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>225</v>
@@ -3861,7 +3770,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -3874,19 +3783,19 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>225</v>
@@ -3941,8 +3850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G61" sqref="G61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>